<commit_message>
added thermocouple connector link
</commit_message>
<xml_diff>
--- a/electronics/sensor-board/sensor-board BOM.xlsx
+++ b/electronics/sensor-board/sensor-board BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NicksFiles\Documents\Penn State\Rocketry\repos\avionics\electronics\sensor-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9405157E-52B6-4E1D-904E-18C6DE8E767A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA416474-1F4E-4303-9A9C-5CCC95F5A8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{505F83C6-C122-45A2-BBF9-74BC7C5786B2}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="163">
   <si>
     <t>Id</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>4 pin molex</t>
+  </si>
+  <si>
+    <t>Thermocouple PCB connector</t>
+  </si>
+  <si>
+    <t>https://evosensors.com/collections/miniature-pcb-flat-mounting/products/k1x-femx-con-fp-x-pccx</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1101,7 @@
   <dimension ref="D4:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1210,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>74</v>
+        <v>161</v>
+      </c>
+      <c r="H12" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.25">

</xml_diff>